<commit_message>
update new map v3
update new map v3
</commit_message>
<xml_diff>
--- a/Regresi Final.xlsx
+++ b/Regresi Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TA\CalibOmni2\sena2024_ws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3F845F-BDBB-436C-A3AD-4F89A7E1AD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D96D451-C97E-4ED2-B51F-BCF7F69165AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A0025BA-1BB6-471B-87C1-5F20766054B8}"/>
   </bookViews>
@@ -1424,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED75AFBC-EC31-4A7C-BA3B-6196784A9209}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>